<commit_message>
Eerste versie presentaties en wijzigingen
</commit_message>
<xml_diff>
--- a/Opdrachten-schema.xlsx
+++ b/Opdrachten-schema.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="28">
   <si>
     <t>Opdrachten om te maken</t>
   </si>
@@ -35,6 +35,9 @@
     <t>Beschrijving</t>
   </si>
   <si>
+    <t>Persoon</t>
+  </si>
+  <si>
     <t>Intro opdracht</t>
   </si>
   <si>
@@ -99,6 +102,12 @@
   </si>
   <si>
     <t>Component maken met simpele String parameter</t>
+  </si>
+  <si>
+    <t>Jeroen</t>
+  </si>
+  <si>
+    <t>Laura</t>
   </si>
 </sst>
 </file>
@@ -419,10 +428,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C11"/>
+  <dimension ref="A1:D11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C11" sqref="C11"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="A11" sqref="A11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -434,12 +443,12 @@
     <col min="5" max="5" width="12.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>1</v>
       </c>
@@ -447,86 +456,113 @@
         <v>2</v>
       </c>
       <c r="C3" t="s">
+        <v>10</v>
+      </c>
+      <c r="D3" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" ht="46.8" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>4</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C4" t="s">
+        <v>11</v>
+      </c>
+      <c r="D4" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" ht="52.8" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>6</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D5" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" ht="51.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>8</v>
+      </c>
+      <c r="B6" s="1" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="4" spans="1:3" ht="46.8" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A4" t="s">
-        <v>3</v>
-      </c>
-      <c r="B4" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="C4" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" ht="52.8" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A5" t="s">
-        <v>5</v>
-      </c>
-      <c r="B5" s="1" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" ht="51.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A6" t="s">
-        <v>7</v>
-      </c>
-      <c r="B6" s="1" t="s">
-        <v>8</v>
-      </c>
       <c r="C6" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
+        <v>12</v>
+      </c>
+      <c r="D6" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
+        <v>14</v>
+      </c>
+      <c r="D7" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="C8" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
+        <v>17</v>
+      </c>
+      <c r="D8" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="C9" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
+        <v>20</v>
+      </c>
+      <c r="D9" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="C10" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
+        <v>23</v>
+      </c>
+      <c r="D10" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>24</v>
+        <v>25</v>
+      </c>
+      <c r="D11" t="s">
+        <v>26</v>
       </c>
     </row>
   </sheetData>

</xml_diff>